<commit_message>
Fixed the mutually exclusiveness of regular and micro-clone process.
</commit_message>
<xml_diff>
--- a/Results of BugReplicationMicroRegularCloneDeckard.xlsx
+++ b/Results of BugReplicationMicroRegularCloneDeckard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Judith\Dropbox\BugReplicationMicroRegularCloneDeckard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6F9AF-6541-47FC-A47F-6A9A1EDD8E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298CBA76-FE3F-48D5-91CE-68F5DCB62618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="1335" windowWidth="16560" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14565" yWindow="5490" windowWidth="13395" windowHeight="7350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>Regular Clones</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>CFs</t>
+  </si>
+  <si>
+    <t>No of Rep bugs</t>
+  </si>
+  <si>
+    <t>No of bugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% </t>
+  </si>
+  <si>
+    <t>No of Severe Rep bugs</t>
   </si>
 </sst>
 </file>
@@ -406,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -524,24 +536,24 @@
         <v>2886</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1592</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E6">
         <f>C6/D6</f>
-        <v>0</v>
+        <v>21.80821917808219</v>
       </c>
       <c r="F6">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="G6">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="H6">
         <f>F6/G6</f>
-        <v>18.551724137931036</v>
+        <v>7.3013698630136989</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -575,27 +587,27 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>1208</v>
+        <v>2800</v>
       </c>
       <c r="D8">
         <f>SUM(D3:D7)</f>
-        <v>230</v>
+        <v>274</v>
       </c>
       <c r="E8">
         <f>C8/D8</f>
-        <v>5.2521739130434781</v>
+        <v>10.218978102189782</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="G8">
         <f>SUM(G3:G7)</f>
-        <v>230</v>
+        <v>274</v>
       </c>
       <c r="H8">
         <f>F8/G8</f>
-        <v>3.534782608695652</v>
+        <v>2.948905109489051</v>
       </c>
     </row>
   </sheetData>
@@ -611,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541805F7-888C-4845-936B-7C5DBFDC2D0B}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,26 +733,50 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="e">
+      <c r="B6">
+        <v>1592</v>
+      </c>
+      <c r="C6">
+        <v>73090</v>
+      </c>
+      <c r="D6">
         <f>B6/C6*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" t="e">
+        <v>2.1781365439868656</v>
+      </c>
+      <c r="E6">
+        <v>533</v>
+      </c>
+      <c r="F6">
+        <v>17942</v>
+      </c>
+      <c r="G6">
         <f>E6/F6*100</f>
-        <v>#DIV/0!</v>
+        <v>2.9706833128971133</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>926</v>
+      </c>
+      <c r="C7">
+        <v>11062</v>
+      </c>
+      <c r="D7">
         <f>B7/C7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>8.3709998192008683</v>
+      </c>
+      <c r="E7">
+        <v>242</v>
+      </c>
+      <c r="F7">
+        <v>1915</v>
+      </c>
+      <c r="G7">
         <f>E7/F7*100</f>
-        <v>#DIV/0!</v>
+        <v>12.637075718015666</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -749,27 +785,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>282</v>
+        <v>2800</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>305</v>
+        <v>84457</v>
       </c>
       <c r="D8">
         <f>B8/C8*100</f>
-        <v>92.459016393442624</v>
+        <v>3.3152965414352864</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>33</v>
+        <v>808</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>41</v>
+        <v>19898</v>
       </c>
       <c r="G8">
         <f>E8/F8*100</f>
-        <v>80.487804878048792</v>
+        <v>4.0607096190571914</v>
       </c>
     </row>
   </sheetData>
@@ -783,24 +819,402 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116FC23D-B249-4D8D-9AE4-0727DADAE3D4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <f>B3/C3*100</f>
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <f>E3/F3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4" si="0">B4/C4*100</f>
+        <v>97.61904761904762</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4" si="1">E4/F4*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="e">
+        <f>B5/C5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" t="e">
+        <f>E5/F5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <v>71</v>
+      </c>
+      <c r="D6">
+        <f>B6/C6*100</f>
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <f>E6/F6*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>117</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7">
+        <f>B7/C7*100</f>
+        <v>95.121951219512198</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <f>E7/F7*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>257</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>264</v>
+      </c>
+      <c r="D8">
+        <f>B8/C8*100</f>
+        <v>97.348484848484844</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v>86</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>86</v>
+      </c>
+      <c r="G8">
+        <f>E8/F8*100</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B70FC0A-4DF8-49BC-AC57-76AAE2965A71}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <f>C3/B3*100</f>
+        <v>32.142857142857146</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <f>F3/E3*100</f>
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4" si="0">C4/B4*100</f>
+        <v>14.634146341463413</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4" si="1">F4/E4*100</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="e">
+        <f>C5/B5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" t="e">
+        <f>F5/E5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <f>C6/B6*100</f>
+        <v>16.901408450704224</v>
+      </c>
+      <c r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f>F6/E6*100</f>
+        <v>7.4074074074074066</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>117</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <f>C7/B7*100</f>
+        <v>16.239316239316238</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <f>F7/E7*100</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>257</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>46</v>
+      </c>
+      <c r="D8">
+        <f>C8/B8*100</f>
+        <v>17.898832684824903</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v>86</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <f>F8/E8*100</f>
+        <v>19.767441860465116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Executing new implementation of readFile().
</commit_message>
<xml_diff>
--- a/Results of BugReplicationMicroRegularCloneDeckard.xlsx
+++ b/Results of BugReplicationMicroRegularCloneDeckard.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Judith\Dropbox\BugReplicationMicroRegularCloneDeckard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298CBA76-FE3F-48D5-91CE-68F5DCB62618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB56D6AB-C1C3-4BDB-934E-22A44D8CD3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14565" yWindow="5490" windowWidth="13395" windowHeight="7350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10290" yWindow="8385" windowWidth="16830" windowHeight="5865" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
     <sheet name="RQ2" sheetId="2" r:id="rId2"/>
     <sheet name="RQ3" sheetId="3" r:id="rId3"/>
     <sheet name="RQ4" sheetId="4" r:id="rId4"/>
+    <sheet name="RQ1a" sheetId="8" r:id="rId5"/>
+    <sheet name="RQ2a" sheetId="9" r:id="rId6"/>
+    <sheet name="RQ3a" sheetId="10" r:id="rId7"/>
+    <sheet name="RQ4a" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="17">
   <si>
     <t>Regular Clones</t>
   </si>
@@ -419,7 +423,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541805F7-888C-4845-936B-7C5DBFDC2D0B}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +826,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1027,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,4 +1221,620 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1405FB40-0315-4C76-9570-BEA6E728A634}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1126</v>
+      </c>
+      <c r="E3" t="e">
+        <f>C3/D3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" t="e">
+        <f>F3/G3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="e">
+        <f t="shared" ref="E4" si="0">C4/D4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" t="e">
+        <f t="shared" ref="H4" si="1">F4/G4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="e">
+        <f>C5/D5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" t="e">
+        <f>F5/G5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2886</v>
+      </c>
+      <c r="E6" t="e">
+        <f>C6/D6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" t="e">
+        <f>F6/G6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="e">
+        <f>C7/D7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="e">
+        <f>F7/G7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D3:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" t="e">
+        <f>C8/D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G3:G7)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="e">
+        <f>F8/G8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894050F4-0FBC-4CD2-8411-14D987BDB292}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>82</v>
+      </c>
+      <c r="C3">
+        <v>88</v>
+      </c>
+      <c r="D3">
+        <f>B3/C3*100</f>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <f>E3/F3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="e">
+        <f t="shared" ref="D4" si="0">B4/C4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" ref="G4" si="1">E4/F4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="e">
+        <f>B5/C5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" t="e">
+        <f>E5/F5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="e">
+        <f>B6/C6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" t="e">
+        <f>E6/F6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="e">
+        <f>B7/C7*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" t="e">
+        <f>E7/F7*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>82</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>88</v>
+      </c>
+      <c r="D8">
+        <f>B8/C8*100</f>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <f>E8/F8*100</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2818F23-3D62-4C3B-9A45-9C5D85ED812B}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="e">
+        <f>B3/C3*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
+        <f>E3/F3*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="e">
+        <f t="shared" ref="D4" si="0">B4/C4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" ref="G4" si="1">E4/F4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="e">
+        <f>B5/C5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" t="e">
+        <f>E5/F5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="e">
+        <f>B6/C6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" t="e">
+        <f>E6/F6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="e">
+        <f>B7/C7*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" t="e">
+        <f>E7/F7*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="e">
+        <f>B8/C8*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
+        <f>E8/F8*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3253A476-F66C-4D2E-BF1B-4E9CEAB8C2CE}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="e">
+        <f>C3/B3*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
+        <f>F3/E3*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="e">
+        <f t="shared" ref="D4" si="0">C4/B4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" ref="G4" si="1">F4/E4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="e">
+        <f>C5/B5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" t="e">
+        <f>F5/E5*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="e">
+        <f>C6/B6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" t="e">
+        <f>F6/E6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="e">
+        <f>C7/B7*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" t="e">
+        <f>F7/E7*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="e">
+        <f>C8/B8*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
+        <f>F8/E8*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>